<commit_message>
cleaning up public files...
</commit_message>
<xml_diff>
--- a/delong-github-public-files-database.xlsx
+++ b/delong-github-public-files-database.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="174">
   <si>
     <t>Table 1</t>
   </si>
@@ -31,426 +31,441 @@
     <t>Course</t>
   </si>
   <si>
-    <t>1919-inevitability-&amp;-chance.pdf</t>
+    <t>2020-03-16-17.04.37-Econ-115-Zoom-594152890=coronavirus.zip</t>
+  </si>
+  <si>
+    <t>lecture q&amp;a zoom session</t>
+  </si>
+  <si>
+    <t>econ-115</t>
+  </si>
+  <si>
+    <t>#tceh</t>
+  </si>
+  <si>
+    <t>2020-03-17-09.55.13-Econ-135-Zoom-7584227890-convergence.zip</t>
+  </si>
+  <si>
+    <t>econ-135</t>
+  </si>
+  <si>
+    <t>2020-03-18-17.00.52-Econ-115-Zoom-594152890.zip</t>
+  </si>
+  <si>
+    <t>article-clark-reading-note.pptx</t>
+  </si>
+  <si>
+    <t>article-dasgupta-reading-note.pptx</t>
+  </si>
+  <si>
+    <t>article-diamond-reading-note.pptx</t>
+  </si>
+  <si>
+    <t>#ieh</t>
+  </si>
+  <si>
+    <t>article-diamond-mistake-reading-note.pptx</t>
+  </si>
+  <si>
+    <t>article-jones-r-&amp;-d-reading-note.pptx</t>
+  </si>
+  <si>
+    <t>article-pritchett-reading-note.pptx</t>
+  </si>
+  <si>
+    <t>article-steckel-reading-note.pptx</t>
+  </si>
+  <si>
+    <t>book-gilgamesh-reading-note.pptx</t>
+  </si>
+  <si>
+    <t>book-selections-clark-farewell-reading-note.pptx</t>
+  </si>
+  <si>
+    <t>book-selections-temin-reading-note.pptx</t>
+  </si>
+  <si>
+    <t>coronavirus-state.xlsx</t>
+  </si>
+  <si>
+    <t>state-by-state coronavirus numbers</t>
+  </si>
+  <si>
+    <t>#corona</t>
+  </si>
+  <si>
+    <t>coronavirus.pptx</t>
+  </si>
+  <si>
+    <t>slides on coronavirus</t>
+  </si>
+  <si>
+    <t>delong-baumol-archive.pdf</t>
+  </si>
+  <si>
+    <t>my 1988 anti-convergence are article</t>
+  </si>
+  <si>
+    <t>delong-github-public-files-database</t>
+  </si>
+  <si>
+    <t>master file &amp; record for things in this directory</t>
+  </si>
+  <si>
+    <t>#index</t>
+  </si>
+  <si>
+    <t>Econ 210a Spring 2020 Syllabus.pdf</t>
+  </si>
+  <si>
+    <t>DEPRECATED—replaced by econ-210a-syllabus.pdf</t>
+  </si>
+  <si>
+    <t>econ-210a</t>
+  </si>
+  <si>
+    <t>econ-115-lecture-1.pptx</t>
+  </si>
+  <si>
+    <t>introduction &amp; themes</t>
+  </si>
+  <si>
+    <t>.pdf</t>
+  </si>
+  <si>
+    <t>econ-115-lecture-10.pptx</t>
+  </si>
+  <si>
+    <t>cold war</t>
+  </si>
+  <si>
+    <t>econ-115-lecture-11.pptx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">false (&amp; true) starts to convergence in emerging markets </t>
+  </si>
+  <si>
+    <t>econ-115-lecture-12.pptx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thirty glorious years, 1945–1975 </t>
+  </si>
+  <si>
+    <t>econ-115-lecture-13.pptx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">social democracy: high tide &amp; ebb </t>
+  </si>
+  <si>
+    <t>econ-115-lecture-14.pptx</t>
+  </si>
+  <si>
+    <t>the end of really existing socialism</t>
+  </si>
+  <si>
+    <t>econ-115-lecture-15.pptx</t>
+  </si>
+  <si>
+    <t>the neoliberal turn (also lecture-neoliberal-turn-text.pdf)</t>
+  </si>
+  <si>
+    <t>#heg</t>
+  </si>
+  <si>
+    <t>econ-115-lecture-2.pptx</t>
+  </si>
+  <si>
+    <t>the watershed: globalization, &amp; the engine of growth</t>
+  </si>
+  <si>
+    <t>econ-115-lecture-3.pptx</t>
+  </si>
+  <si>
+    <t>north atlantic political economy 1870-1914</t>
+  </si>
+  <si>
+    <t>econ-115-lecture-4.pptx</t>
+  </si>
+  <si>
+    <t>empire &amp; war</t>
+  </si>
+  <si>
+    <t>econ-115-lecture-5.pptx</t>
+  </si>
+  <si>
+    <t>trying to rebuild civilization after www</t>
+  </si>
+  <si>
+    <t>econ-115-lecture-6.pptx</t>
+  </si>
+  <si>
+    <t>macroeconomic for beginners &amp; roaring twenties</t>
+  </si>
+  <si>
+    <t>econ-115-lecture-7.pptx</t>
+  </si>
+  <si>
+    <t>understanding the great depression</t>
+  </si>
+  <si>
+    <t>econ-115-lecture-8.pptx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alternatives to let-it-alone marketism </t>
+  </si>
+  <si>
+    <t>econ-115-lecture-9.pptx</t>
+  </si>
+  <si>
+    <t>fascism &amp; wwii</t>
+  </si>
+  <si>
+    <t>econ-135-changeup-review-2-5-10-20.pptx</t>
+  </si>
+  <si>
+    <t>pre-midterm review</t>
+  </si>
+  <si>
+    <t>econ-135-lecture-1.pptx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the big picture: economic growth in historical perspective </t>
+  </si>
+  <si>
+    <t>econ-135-lecture-10.pptx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the industrial revolution ii </t>
+  </si>
+  <si>
+    <t>econ-135-lecture-11.pptx</t>
+  </si>
+  <si>
+    <t>why northwest europe?</t>
+  </si>
+  <si>
+    <t>econ-135-lecture-12.pptx</t>
+  </si>
+  <si>
+    <t>modern economic growth</t>
+  </si>
+  <si>
+    <t>econ-135-lecture-13.pptx</t>
+  </si>
+  <si>
+    <t>u.s. economic ascendancy (also: how america became the exceptional nation)</t>
+  </si>
+  <si>
+    <t>econ-135-lecture-14.pptx</t>
+  </si>
+  <si>
+    <t>globalization advances &amp; retreats</t>
+  </si>
+  <si>
+    <t>econ-135-lecture-15.pptx</t>
+  </si>
+  <si>
+    <t>convergence &amp; its absence</t>
+  </si>
+  <si>
+    <t>econ-135-lecture-16.pptx</t>
+  </si>
+  <si>
+    <t>inequality &amp; plutocracy (also: lecture-inequality.pptx, lecture-inequality-text.pdf</t>
+  </si>
+  <si>
+    <t>econ-135-lecture-17.pptx</t>
+  </si>
+  <si>
+    <t>the development of underdevelopment: explication of lewis: evolution</t>
+  </si>
+  <si>
+    <t>econ-135-lecture-2-outline-solow-theory.pptx</t>
+  </si>
+  <si>
+    <t>outline &amp; cheat sheet for the solow growth model</t>
+  </si>
+  <si>
+    <t>econ-135-lecture-2.pptx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">theory: robert solow’s economic growth model </t>
+  </si>
+  <si>
+    <t>econ-135-lecture-3-outline-malthusian-theory.pptx</t>
+  </si>
+  <si>
+    <t>outline &amp; cheat sheet for the malthusian growth model</t>
+  </si>
+  <si>
+    <t>econ-135-lecture-3.pptx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">theory: the malthus-solow economic growth model </t>
+  </si>
+  <si>
+    <t>econ-135-lecture-4.pptx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">theory: determinants of the rate of growth </t>
+  </si>
+  <si>
+    <t>econ-135-lecture-5.pptx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intensive economic growth’s absence in the malthusian agrarian age </t>
+  </si>
+  <si>
+    <t>econ-135-lecture-6.pptx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ancient empires: “efflorescences”, rises, &amp; falls </t>
+  </si>
+  <si>
+    <t>econ-135-lecture-7.pptx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">why was pre-industrial progress so slow on average? </t>
+  </si>
+  <si>
+    <t>econ-135-lecture-8.pptx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">commercial revolutions </t>
+  </si>
+  <si>
+    <t>econ-135-lecture-9.pptx</t>
+  </si>
+  <si>
+    <t>the industrial revolution i</t>
+  </si>
+  <si>
+    <t>econ-210a-lecture-1.pptx</t>
+  </si>
+  <si>
+    <t>introduction to economic history &amp; malthusian economies</t>
+  </si>
+  <si>
+    <t>econ-210a-lecture-1a.pptx</t>
+  </si>
+  <si>
+    <t>introduction to economic history</t>
+  </si>
+  <si>
+    <t>econ-210a-lecture-1b.pptx</t>
+  </si>
+  <si>
+    <t>malthusian economies</t>
+  </si>
+  <si>
+    <t>econ-210a-lecture-2.pptx</t>
+  </si>
+  <si>
+    <t>technology &amp; organization in the very long run</t>
+  </si>
+  <si>
+    <t>econ-210a-lecture-2a.pptx</t>
+  </si>
+  <si>
+    <t>econ-210a-lecture-2b.pptx</t>
+  </si>
+  <si>
+    <t>commercial revolutions</t>
+  </si>
+  <si>
+    <t>econ-210a-lecture-3a.pptx</t>
+  </si>
+  <si>
+    <t>econ-210a-lecture-3b.pptx</t>
+  </si>
+  <si>
+    <t>industrial revolutions</t>
+  </si>
+  <si>
+    <t>econ-210a-lecture-4a.pptx</t>
+  </si>
+  <si>
+    <t>econ-210a-lecture-4b.pptx</t>
+  </si>
+  <si>
+    <t>comparative development &amp; underdevelopment</t>
+  </si>
+  <si>
+    <t>econ-210a-lecture-5a.pptx</t>
+  </si>
+  <si>
+    <t>econ-210a-lecture-5b.pptx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modern economic growth </t>
+  </si>
+  <si>
+    <t>econ-210a-lecture-6a.pptx</t>
+  </si>
+  <si>
+    <t>econ-210a-lecture-6b.pptx</t>
+  </si>
+  <si>
+    <t>unfreedom</t>
+  </si>
+  <si>
+    <t>econ-210a-lecture-8a.pptx</t>
+  </si>
+  <si>
+    <t>econ-210a-lecture-8b.pptx</t>
+  </si>
+  <si>
+    <t>women, men, &amp; children</t>
+  </si>
+  <si>
+    <t>econ-210a-lecture-9a.pptx</t>
+  </si>
+  <si>
+    <t>capital markets</t>
+  </si>
+  <si>
+    <t>econ-210a-syllabus.pdf</t>
+  </si>
+  <si>
+    <t>updated syllabus &amp; reading list to graduate introduction to economic history course</t>
+  </si>
+  <si>
+    <t>book-selections-evans-embedded-i.pdf</t>
+  </si>
+  <si>
+    <t>peter evens: embedded autonomy—ch 1 of the go-to book on industrial policy</t>
+  </si>
+  <si>
+    <t>econ-hist-grad-intro.pdf</t>
+  </si>
+  <si>
+    <t>syllabus &amp; reading list to graduate introduction to economic history course</t>
+  </si>
+  <si>
+    <t>ps-judy-shelton-2020-03.pdf</t>
+  </si>
+  <si>
+    <t>importance of preserving technocratic chops of the fed</t>
+  </si>
+  <si>
+    <t>#ps</t>
+  </si>
+  <si>
+    <t>#ohb</t>
+  </si>
+  <si>
+    <t>lecture-1919-inevitability-&amp;-chance.pdf</t>
   </si>
   <si>
     <t>wwi &amp; its outcome as a butterfly-flap crux of history</t>
   </si>
   <si>
-    <t>econ-115</t>
-  </si>
-  <si>
-    <t>#tceh</t>
-  </si>
-  <si>
-    <t>2020-03-16-17.04.37-Econ-115-Zoom-594152890=coronavirus.zip</t>
-  </si>
-  <si>
-    <t>lecture q&amp;a zoom session</t>
-  </si>
-  <si>
-    <t>2020-03-17-09.55.13-Econ-135-Zoom-7584227890-convergence.zip</t>
-  </si>
-  <si>
-    <t>econ-135</t>
-  </si>
-  <si>
-    <t>2020-03-18-17.00.52-Econ-115-Zoom-594152890.zip</t>
-  </si>
-  <si>
-    <t>american-exceptionalism-#TCEH.pdf</t>
+    <t>lecture-american-exceptionalism.pdf</t>
   </si>
   <si>
     <t>how america became the exceptional nation in the long 20th century (econ-135-lecture-13.pptx)</t>
   </si>
   <si>
-    <t>#heg</t>
-  </si>
-  <si>
-    <t>article-clark-reading-note.pptx</t>
-  </si>
-  <si>
-    <t>article-dasgupta-reading-note.pptx</t>
-  </si>
-  <si>
-    <t>article-diamond-#ieh.pptx</t>
-  </si>
-  <si>
-    <t>article-diamond-mistake-reading-note.pptx</t>
-  </si>
-  <si>
-    <t>article-jones-r-&amp;-d.pptx</t>
-  </si>
-  <si>
-    <t>article-pritchett-reading-note.pptx</t>
-  </si>
-  <si>
-    <t>article-steckel.pptx</t>
-  </si>
-  <si>
-    <t>book-gilgamesh-reading-note.pptx</t>
-  </si>
-  <si>
-    <t>book-selections-clark-farewell-#ieh.pptx</t>
-  </si>
-  <si>
-    <t>book-temin-selections-reading-note.pptx</t>
-  </si>
-  <si>
-    <t>coronavirus-state.xlsx</t>
-  </si>
-  <si>
-    <t>state-by-state coronavirus numbers</t>
-  </si>
-  <si>
-    <t>#corona</t>
-  </si>
-  <si>
-    <t>coronavirus.pptx</t>
-  </si>
-  <si>
-    <t>slides on coronavirus</t>
-  </si>
-  <si>
-    <t>delong-baumol.pdf</t>
-  </si>
-  <si>
-    <t>my 1988 anti-convergence are article</t>
-  </si>
-  <si>
-    <t>Econ 210a Spring 2020 Syllabus.pdf</t>
-  </si>
-  <si>
-    <t>DEPRECATED—replaced by econ-210a-syllabus.pdf</t>
-  </si>
-  <si>
-    <t>econ-210a</t>
-  </si>
-  <si>
-    <t>#ieh</t>
-  </si>
-  <si>
-    <t>econ-115-lecture-1.pptx</t>
-  </si>
-  <si>
-    <t>introduction &amp; themes</t>
-  </si>
-  <si>
-    <t>.pdf</t>
-  </si>
-  <si>
-    <t>econ-115-lecture-10.pptx</t>
-  </si>
-  <si>
-    <t>cold war</t>
-  </si>
-  <si>
-    <t>econ-115-lecture-11.pptx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">false (&amp; true) starts to convergence in emerging markets </t>
-  </si>
-  <si>
-    <t>econ-115-lecture-12.pptx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">thirty glorious years, 1945–1975 </t>
-  </si>
-  <si>
-    <t>econ-115-lecture-13.pptx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">social democracy: high tide &amp; ebb </t>
-  </si>
-  <si>
-    <t>econ-115-lecture-14.pptx</t>
-  </si>
-  <si>
-    <t>the end of really existing socialism</t>
-  </si>
-  <si>
-    <t>econ-115-lecture-2.pptx</t>
-  </si>
-  <si>
-    <t>the watershed: globalization, &amp; the engine of growth</t>
-  </si>
-  <si>
-    <t>econ-115-lecture-3.pptx</t>
-  </si>
-  <si>
-    <t>north atlantic political economy 1870-1914</t>
-  </si>
-  <si>
-    <t>econ-115-lecture-4.pptx</t>
-  </si>
-  <si>
-    <t>empire &amp; war</t>
-  </si>
-  <si>
-    <t>econ-115-lecture-5.pptx</t>
-  </si>
-  <si>
-    <t>trying to rebuild civilization after www</t>
-  </si>
-  <si>
-    <t>econ-115-lecture-6.pptx</t>
-  </si>
-  <si>
-    <t>macroeconomic for beginners &amp; roaring twenties</t>
-  </si>
-  <si>
-    <t>econ-115-lecture-7.pptx</t>
-  </si>
-  <si>
-    <t>understanding the great depression</t>
-  </si>
-  <si>
-    <t>econ-115-lecture-8.pptx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alternatives to let-it-alone marketism </t>
-  </si>
-  <si>
-    <t>econ-115-lecture-9.pptx</t>
-  </si>
-  <si>
-    <t>fascism &amp; wwii</t>
-  </si>
-  <si>
-    <t>econ-135-changeup-review-2-5-10-20.pptx</t>
-  </si>
-  <si>
-    <t>pre-midterm review</t>
-  </si>
-  <si>
-    <t>econ-135-lecture-1.pptx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">the big picture: economic growth in historical perspective </t>
-  </si>
-  <si>
-    <t>econ-135-lecture-10.pptx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">the industrial revolution ii </t>
-  </si>
-  <si>
-    <t>econ-135-lecture-11.pptx</t>
-  </si>
-  <si>
-    <t>why northwest europe?</t>
-  </si>
-  <si>
-    <t>econ-135-lecture-12.pptx</t>
-  </si>
-  <si>
-    <t>modern economic growth</t>
-  </si>
-  <si>
-    <t>econ-135-lecture-13.pptx</t>
-  </si>
-  <si>
-    <t>u.s. economic ascendancy (also: how america became the exceptional nation)</t>
-  </si>
-  <si>
-    <t>econ-135-lecture-14.pptx</t>
-  </si>
-  <si>
-    <t>globalization advances &amp; retreats</t>
-  </si>
-  <si>
-    <t>econ-135-lecture-15.pptx</t>
-  </si>
-  <si>
-    <t>convergence &amp; its absence</t>
-  </si>
-  <si>
-    <t>econ-135-lecture-16.pptx</t>
-  </si>
-  <si>
-    <t>inequality &amp; plutocracy (also: lecture-inequality.pptx, lecture-inequality-text.pdf</t>
-  </si>
-  <si>
-    <t>econ-135-lecture-17.pptx</t>
-  </si>
-  <si>
-    <t>the development of underdevelopment: explication of lewis: evolution</t>
-  </si>
-  <si>
-    <t>econ-135-lecture-2-outline-solow-theory.pptx</t>
-  </si>
-  <si>
-    <t>outline &amp; cheat sheet for the solow growth model</t>
-  </si>
-  <si>
-    <t>econ-135-lecture-2.pptx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">theory: robert solow’s economic growth model </t>
-  </si>
-  <si>
-    <t>econ-135-lecture-3-outline-malthusian-theory.pptx</t>
-  </si>
-  <si>
-    <t>outline &amp; cheat sheet for the malthusian growth model</t>
-  </si>
-  <si>
-    <t>econ-135-lecture-3.pptx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">theory: the malthus-solow economic growth model </t>
-  </si>
-  <si>
-    <t>econ-135-lecture-4.pptx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">theory: determinants of the rate of growth </t>
-  </si>
-  <si>
-    <t>econ-135-lecture-5.pptx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">intensive economic growth’s absence in the malthusian agrarian age </t>
-  </si>
-  <si>
-    <t>econ-135-lecture-6.pptx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ancient empires: “efflorescences”, rises, &amp; falls </t>
-  </si>
-  <si>
-    <t>econ-135-lecture-7.pptx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">why was pre-industrial progress so slow on average? </t>
-  </si>
-  <si>
-    <t>econ-135-lecture-8.pptx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">commercial revolutions </t>
-  </si>
-  <si>
-    <t>econ-135-lecture-9.pptx</t>
-  </si>
-  <si>
-    <t>the industrial revolution i</t>
-  </si>
-  <si>
-    <t>econ-210a-lecture-1.pptx</t>
-  </si>
-  <si>
-    <t>introduction to economic history &amp; malthusian economies</t>
-  </si>
-  <si>
-    <t>econ-210a-lecture-1a.pptx</t>
-  </si>
-  <si>
-    <t>introduction to economic history</t>
-  </si>
-  <si>
-    <t>econ-210a-lecture-1b.pptx</t>
-  </si>
-  <si>
-    <t>malthusian economies</t>
-  </si>
-  <si>
-    <t>econ-210a-lecture-2.pptx</t>
-  </si>
-  <si>
-    <t>technology &amp; organization in the very long run</t>
-  </si>
-  <si>
-    <t>econ-210a-lecture-2a.pptx</t>
-  </si>
-  <si>
-    <t>econ-210a-lecture-2b.pptx</t>
-  </si>
-  <si>
-    <t>commercial revolutions</t>
-  </si>
-  <si>
-    <t>econ-210a-lecture-3a.pptx</t>
-  </si>
-  <si>
-    <t>econ-210a-lecture-3b.pptx</t>
-  </si>
-  <si>
-    <t>industrial revolutions</t>
-  </si>
-  <si>
-    <t>econ-210a-lecture-4a.pptx</t>
-  </si>
-  <si>
-    <t>econ-210a-lecture-4b.pptx</t>
-  </si>
-  <si>
-    <t>comparative development &amp; underdevelopment</t>
-  </si>
-  <si>
-    <t>econ-210a-lecture-5a.pptx</t>
-  </si>
-  <si>
-    <t>econ-210a-lecture-5b.pptx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">modern economic growth </t>
-  </si>
-  <si>
-    <t>econ-210a-lecture-6a.pptx</t>
-  </si>
-  <si>
-    <t>econ-210a-lecture-6b.pptx</t>
-  </si>
-  <si>
-    <t>unfreedom</t>
-  </si>
-  <si>
-    <t>econ-210a-lecture-8a.pptx</t>
-  </si>
-  <si>
-    <t>econ-210a-lecture-8b.pptx</t>
-  </si>
-  <si>
-    <t>women, men, &amp; children</t>
-  </si>
-  <si>
-    <t>econ-210a-lecture-9a.pptx</t>
-  </si>
-  <si>
-    <t>capital markets</t>
-  </si>
-  <si>
-    <t>econ-210a-syllabus.pdf</t>
-  </si>
-  <si>
-    <t>updated syllabus &amp; reading list to graduate introduction to economic history course</t>
-  </si>
-  <si>
-    <t>evans-embedded-i.pdf</t>
-  </si>
-  <si>
-    <t>peter evens: embedded autonomy—ch 1 of the go-to book on industrial policy</t>
-  </si>
-  <si>
-    <t>intro-econ-hist-grad.pdf</t>
-  </si>
-  <si>
-    <t>syllabus &amp; reading list to graduate introduction to economic history course</t>
-  </si>
-  <si>
-    <t>judy-shelton-project-syndicate-2020-03.pdf</t>
-  </si>
-  <si>
-    <t>importance of preserving technocratic chops of the fed</t>
-  </si>
-  <si>
-    <t>#ps</t>
-  </si>
-  <si>
-    <t>#ohb</t>
-  </si>
-  <si>
     <t>lecture-development-of-underdevelopment-text.pdf</t>
   </si>
   <si>
@@ -469,7 +484,13 @@
     <t>invited lecture (brown)—slides (also text available)</t>
   </si>
   <si>
-    <t>lewis-evolution-a.pdf</t>
+    <t>lecture-neoliberal-turn-text.pdf</t>
+  </si>
+  <si>
+    <t>the neoliberal turn (also econ-115-lecture-15.pptx)</t>
+  </si>
+  <si>
+    <t>book-lewis-evolution-a.pdf</t>
   </si>
   <si>
     <t>w. arthur lewis: evolution of the international economic order i</t>
@@ -478,7 +499,7 @@
     <t>#read</t>
   </si>
   <si>
-    <t>lewis-evolution-b.pdf</t>
+    <t>book-lewis-evolution-b.pdf</t>
   </si>
   <si>
     <t>w. arthur lewis: evolution of the international economic order ii</t>
@@ -493,13 +514,13 @@
     <t>module-malthusian-#MRE-d.pptx</t>
   </si>
   <si>
-    <t>neoliberalism.pptx</t>
+    <t>lecture-neoliberalism.pptx</t>
   </si>
   <si>
     <t>neoliberalism, state capacity, &amp; economic growth &amp; development: invited skema lecture</t>
   </si>
   <si>
-    <t>reading-robert-allen-ir.pptx</t>
+    <t>book-robert-allen-ir-reading-note.pptx</t>
   </si>
   <si>
     <t>us-coronavirus-deaths.xlsx</t>
@@ -508,16 +529,10 @@
     <t>u.s. coronavirus deaths by date</t>
   </si>
   <si>
-    <t>wealth-tax-project-syndicate-2020-02.pdf</t>
+    <t>ps-wealth-tax-2020-02.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">decision between wealth, income, consumption taxes should be based on convenience of implementation </t>
-  </si>
-  <si>
-    <t>delong-github-public-files-database</t>
-  </si>
-  <si>
-    <t>master file &amp; record for things in this directory</t>
   </si>
 </sst>
 </file>
@@ -1813,7 +1828,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:L89"/>
+  <dimension ref="A2:M91"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
@@ -1827,8 +1842,8 @@
     <col min="6" max="6" width="7.28906" style="1" customWidth="1"/>
     <col min="7" max="7" width="6.86719" style="1" customWidth="1"/>
     <col min="8" max="8" width="8.70312" style="1" customWidth="1"/>
-    <col min="9" max="12" width="6.86719" style="1" customWidth="1"/>
-    <col min="13" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="9" max="13" width="6.86719" style="1" customWidth="1"/>
+    <col min="14" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
@@ -1846,6 +1861,7 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
       <c r="A2" t="s" s="3">
@@ -1870,6 +1886,7 @@
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
     </row>
     <row r="3" ht="20.25" customHeight="1">
       <c r="A3" t="s" s="5">
@@ -1880,7 +1897,7 @@
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="8">
-        <v>43904</v>
+        <v>43906</v>
       </c>
       <c r="E3" t="s" s="9">
         <v>8</v>
@@ -1894,20 +1911,21 @@
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
       <c r="A4" t="s" s="10">
         <v>10</v>
       </c>
       <c r="B4" t="s" s="11">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="13">
-        <v>43906</v>
+        <v>43907</v>
       </c>
       <c r="E4" t="s" s="14">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s" s="14">
         <v>9</v>
@@ -1918,20 +1936,21 @@
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
       <c r="A5" t="s" s="10">
         <v>12</v>
       </c>
       <c r="B5" t="s" s="11">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="13">
-        <v>43907</v>
+        <v>43908</v>
       </c>
       <c r="E5" t="s" s="14">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s" s="14">
         <v>9</v>
@@ -1942,60 +1961,49 @@
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
       <c r="A6" t="s" s="10">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s" s="11">
-        <v>11</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B6" s="15"/>
       <c r="C6" s="12"/>
       <c r="D6" s="13">
-        <v>43908</v>
-      </c>
-      <c r="E6" t="s" s="14">
-        <v>8</v>
-      </c>
-      <c r="F6" t="s" s="14">
-        <v>9</v>
-      </c>
+        <v>43875</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
       <c r="A7" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s" s="11">
-        <v>16</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B7" s="15"/>
       <c r="C7" s="12"/>
       <c r="D7" s="13">
-        <v>43903</v>
-      </c>
-      <c r="E7" t="s" s="14">
-        <v>13</v>
-      </c>
-      <c r="F7" t="s" s="14">
-        <v>9</v>
-      </c>
-      <c r="G7" t="s" s="14">
-        <v>17</v>
-      </c>
+        <v>43851</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
       <c r="A8" t="s" s="10">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="12"/>
@@ -2006,14 +2014,17 @@
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
+      <c r="I8" t="s" s="14">
+        <v>16</v>
+      </c>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
       <c r="A9" t="s" s="10">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="12"/>
@@ -2024,19 +2035,22 @@
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
+      <c r="I9" t="s" s="14">
+        <v>16</v>
+      </c>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" t="s" s="10">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="12"/>
       <c r="D10" s="13">
-        <v>43875</v>
+        <v>43851</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
@@ -2046,10 +2060,11 @@
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
       <c r="A11" t="s" s="10">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B11" s="15"/>
       <c r="C11" s="12"/>
@@ -2064,15 +2079,16 @@
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
       <c r="A12" t="s" s="10">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="12"/>
       <c r="D12" s="13">
-        <v>43851</v>
+        <v>43875</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
@@ -2082,10 +2098,11 @@
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
       <c r="A13" t="s" s="10">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="12"/>
@@ -2100,10 +2117,11 @@
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
       <c r="A14" t="s" s="10">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="12"/>
@@ -2118,15 +2136,16 @@
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
       <c r="A15" t="s" s="10">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="12"/>
       <c r="D15" s="13">
-        <v>43851</v>
+        <v>43875</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
@@ -2136,64 +2155,74 @@
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
       <c r="A16" t="s" s="10">
-        <v>26</v>
-      </c>
-      <c r="B16" s="15"/>
+        <v>24</v>
+      </c>
+      <c r="B16" t="s" s="11">
+        <v>25</v>
+      </c>
       <c r="C16" s="12"/>
       <c r="D16" s="13">
-        <v>43875</v>
+        <v>43920</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
+      <c r="H16" t="s" s="14">
+        <v>26</v>
+      </c>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
       <c r="A17" t="s" s="10">
         <v>27</v>
       </c>
-      <c r="B17" s="15"/>
+      <c r="B17" t="s" s="11">
+        <v>28</v>
+      </c>
       <c r="C17" s="12"/>
       <c r="D17" s="13">
-        <v>43875</v>
+        <v>43912</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
+      <c r="H17" t="s" s="14">
+        <v>26</v>
+      </c>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
       <c r="A18" t="s" s="10">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s" s="11">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C18" s="12"/>
       <c r="D18" s="13">
-        <v>43920</v>
+        <v>43906</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
-      <c r="H18" t="s" s="14">
-        <v>30</v>
-      </c>
+      <c r="H18" s="12"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
       <c r="A19" t="s" s="10">
@@ -2204,75 +2233,84 @@
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="13">
-        <v>43912</v>
+        <v>43920</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
-      <c r="H19" t="s" s="14">
-        <v>30</v>
-      </c>
+      <c r="H19" s="12"/>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
+      <c r="M19" t="s" s="14">
+        <v>33</v>
+      </c>
     </row>
     <row r="20" ht="20.05" customHeight="1">
       <c r="A20" t="s" s="10">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s" s="11">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C20" s="12"/>
       <c r="D20" s="13">
-        <v>43906</v>
-      </c>
-      <c r="E20" s="12"/>
+        <v>43875</v>
+      </c>
+      <c r="E20" t="s" s="14">
+        <v>36</v>
+      </c>
       <c r="F20" s="12"/>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
+      <c r="I20" t="s" s="14">
+        <v>16</v>
+      </c>
       <c r="J20" s="12"/>
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
       <c r="A21" t="s" s="10">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s" s="11">
-        <v>36</v>
-      </c>
-      <c r="C21" s="12"/>
+        <v>38</v>
+      </c>
+      <c r="C21" t="s" s="14">
+        <v>39</v>
+      </c>
       <c r="D21" s="13">
         <v>43875</v>
       </c>
       <c r="E21" t="s" s="14">
-        <v>37</v>
-      </c>
-      <c r="F21" s="12"/>
+        <v>8</v>
+      </c>
+      <c r="F21" t="s" s="14">
+        <v>9</v>
+      </c>
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
-      <c r="I21" t="s" s="14">
-        <v>38</v>
-      </c>
+      <c r="I21" s="12"/>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
       <c r="A22" t="s" s="10">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B22" t="s" s="11">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D22" s="13">
-        <v>43875</v>
+        <v>43903</v>
       </c>
       <c r="E22" t="s" s="14">
         <v>8</v>
@@ -2286,6 +2324,7 @@
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
     </row>
     <row r="23" ht="20.05" customHeight="1">
       <c r="A23" t="s" s="10">
@@ -2295,7 +2334,7 @@
         <v>43</v>
       </c>
       <c r="C23" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D23" s="13">
         <v>43903</v>
@@ -2312,6 +2351,7 @@
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
     </row>
     <row r="24" ht="20.05" customHeight="1">
       <c r="A24" t="s" s="10">
@@ -2321,7 +2361,7 @@
         <v>45</v>
       </c>
       <c r="C24" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D24" s="13">
         <v>43903</v>
@@ -2338,6 +2378,7 @@
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
     </row>
     <row r="25" ht="20.05" customHeight="1">
       <c r="A25" t="s" s="10">
@@ -2347,10 +2388,10 @@
         <v>47</v>
       </c>
       <c r="C25" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D25" s="13">
-        <v>43903</v>
+        <v>43920</v>
       </c>
       <c r="E25" t="s" s="14">
         <v>8</v>
@@ -2364,6 +2405,7 @@
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
     </row>
     <row r="26" ht="20.05" customHeight="1">
       <c r="A26" t="s" s="10">
@@ -2373,10 +2415,10 @@
         <v>49</v>
       </c>
       <c r="C26" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D26" s="13">
-        <v>43920</v>
+        <v>43916</v>
       </c>
       <c r="E26" t="s" s="14">
         <v>8</v>
@@ -2390,6 +2432,7 @@
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
     </row>
     <row r="27" ht="20.05" customHeight="1">
       <c r="A27" t="s" s="10">
@@ -2399,10 +2442,10 @@
         <v>51</v>
       </c>
       <c r="C27" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D27" s="13">
-        <v>43916</v>
+        <v>43921</v>
       </c>
       <c r="E27" t="s" s="14">
         <v>8</v>
@@ -2410,22 +2453,25 @@
       <c r="F27" t="s" s="14">
         <v>9</v>
       </c>
-      <c r="G27" s="12"/>
+      <c r="G27" t="s" s="14">
+        <v>52</v>
+      </c>
       <c r="H27" s="12"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
       <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
     </row>
     <row r="28" ht="20.05" customHeight="1">
       <c r="A28" t="s" s="10">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B28" t="s" s="11">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C28" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D28" s="13">
         <v>43875</v>
@@ -2442,16 +2488,17 @@
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
       <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
     </row>
     <row r="29" ht="20.05" customHeight="1">
       <c r="A29" t="s" s="10">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B29" t="s" s="11">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C29" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D29" s="13">
         <v>43875</v>
@@ -2468,16 +2515,17 @@
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
       <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
     </row>
     <row r="30" ht="20.05" customHeight="1">
       <c r="A30" t="s" s="10">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B30" t="s" s="11">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C30" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D30" s="13">
         <v>43875</v>
@@ -2494,16 +2542,17 @@
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
       <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
     </row>
     <row r="31" ht="20.05" customHeight="1">
       <c r="A31" t="s" s="10">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B31" t="s" s="11">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C31" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D31" s="13">
         <v>43875</v>
@@ -2520,16 +2569,17 @@
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
       <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
     </row>
     <row r="32" ht="20.05" customHeight="1">
       <c r="A32" t="s" s="10">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B32" t="s" s="11">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C32" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D32" s="13">
         <v>43875</v>
@@ -2546,16 +2596,17 @@
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
       <c r="L32" s="12"/>
+      <c r="M32" s="12"/>
     </row>
     <row r="33" ht="20.05" customHeight="1">
       <c r="A33" t="s" s="10">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B33" t="s" s="11">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C33" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D33" s="13">
         <v>43903</v>
@@ -2572,16 +2623,17 @@
       <c r="J33" s="12"/>
       <c r="K33" s="12"/>
       <c r="L33" s="12"/>
+      <c r="M33" s="12"/>
     </row>
     <row r="34" ht="20.05" customHeight="1">
       <c r="A34" t="s" s="10">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B34" t="s" s="11">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C34" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D34" s="13">
         <v>43903</v>
@@ -2598,16 +2650,17 @@
       <c r="J34" s="12"/>
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
+      <c r="M34" s="12"/>
     </row>
     <row r="35" ht="20.05" customHeight="1">
       <c r="A35" t="s" s="10">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B35" t="s" s="11">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C35" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D35" s="13">
         <v>43903</v>
@@ -2624,999 +2677,1038 @@
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
+      <c r="M35" s="12"/>
     </row>
     <row r="36" ht="20.05" customHeight="1">
       <c r="A36" t="s" s="10">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B36" t="s" s="11">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C36" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D36" s="13">
         <v>43875</v>
       </c>
       <c r="E36" t="s" s="14">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F36" s="12"/>
       <c r="G36" t="s" s="14">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="H36" s="12"/>
       <c r="I36" s="12"/>
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
       <c r="L36" s="12"/>
+      <c r="M36" s="12"/>
     </row>
     <row r="37" ht="20.05" customHeight="1">
       <c r="A37" t="s" s="10">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B37" t="s" s="11">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C37" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D37" s="13">
         <v>43875</v>
       </c>
       <c r="E37" t="s" s="14">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F37" s="12"/>
       <c r="G37" t="s" s="14">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="H37" s="12"/>
       <c r="I37" s="12"/>
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
       <c r="L37" s="12"/>
+      <c r="M37" s="12"/>
     </row>
     <row r="38" ht="20.05" customHeight="1">
       <c r="A38" t="s" s="10">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B38" t="s" s="11">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C38" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D38" s="13">
         <v>43888</v>
       </c>
       <c r="E38" t="s" s="14">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F38" s="12"/>
       <c r="G38" t="s" s="14">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="H38" s="12"/>
       <c r="I38" s="12"/>
       <c r="J38" s="12"/>
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
+      <c r="M38" s="12"/>
     </row>
     <row r="39" ht="20.05" customHeight="1">
       <c r="A39" t="s" s="10">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B39" t="s" s="11">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C39" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D39" s="13">
         <v>43903</v>
       </c>
       <c r="E39" t="s" s="14">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F39" s="12"/>
       <c r="G39" t="s" s="14">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="H39" s="12"/>
       <c r="I39" s="12"/>
       <c r="J39" s="12"/>
       <c r="K39" s="12"/>
       <c r="L39" s="12"/>
+      <c r="M39" s="12"/>
     </row>
     <row r="40" ht="20.05" customHeight="1">
       <c r="A40" t="s" s="10">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B40" t="s" s="11">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C40" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D40" s="13">
         <v>43903</v>
       </c>
       <c r="E40" t="s" s="14">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F40" s="12"/>
       <c r="G40" t="s" s="14">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="H40" s="12"/>
       <c r="I40" s="12"/>
       <c r="J40" s="12"/>
       <c r="K40" s="12"/>
       <c r="L40" s="12"/>
+      <c r="M40" s="12"/>
     </row>
     <row r="41" ht="20.05" customHeight="1">
       <c r="A41" t="s" s="10">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B41" t="s" s="11">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C41" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D41" s="13">
         <v>43903</v>
       </c>
       <c r="E41" t="s" s="14">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F41" s="12"/>
       <c r="G41" t="s" s="14">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="H41" s="12"/>
       <c r="I41" s="12"/>
       <c r="J41" s="12"/>
       <c r="K41" s="12"/>
       <c r="L41" s="12"/>
+      <c r="M41" s="12"/>
     </row>
     <row r="42" ht="20.05" customHeight="1">
       <c r="A42" t="s" s="10">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B42" t="s" s="11">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C42" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D42" s="13">
         <v>43903</v>
       </c>
       <c r="E42" t="s" s="14">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F42" s="12"/>
       <c r="G42" t="s" s="14">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="H42" s="12"/>
       <c r="I42" s="12"/>
       <c r="J42" s="12"/>
       <c r="K42" s="12"/>
       <c r="L42" s="12"/>
+      <c r="M42" s="12"/>
     </row>
     <row r="43" ht="20.05" customHeight="1">
       <c r="A43" t="s" s="10">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B43" t="s" s="11">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C43" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D43" s="13">
         <v>43907</v>
       </c>
       <c r="E43" t="s" s="14">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F43" s="12"/>
       <c r="G43" t="s" s="14">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="H43" s="12"/>
       <c r="I43" s="12"/>
       <c r="J43" s="12"/>
       <c r="K43" s="12"/>
       <c r="L43" s="12"/>
+      <c r="M43" s="12"/>
     </row>
     <row r="44" ht="20.05" customHeight="1">
       <c r="A44" t="s" s="10">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B44" t="s" s="11">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C44" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D44" s="13">
         <v>43909</v>
       </c>
       <c r="E44" t="s" s="14">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F44" s="12"/>
       <c r="G44" t="s" s="14">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="H44" s="12"/>
       <c r="I44" s="12"/>
       <c r="J44" s="12"/>
       <c r="K44" s="12"/>
       <c r="L44" s="12"/>
+      <c r="M44" s="12"/>
     </row>
     <row r="45" ht="20.05" customHeight="1">
       <c r="A45" t="s" s="10">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B45" t="s" s="11">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C45" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D45" s="13">
         <v>43919</v>
       </c>
       <c r="E45" t="s" s="14">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F45" s="12"/>
       <c r="G45" t="s" s="14">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="H45" s="12"/>
       <c r="I45" s="12"/>
       <c r="J45" s="12"/>
       <c r="K45" s="12"/>
       <c r="L45" s="12"/>
+      <c r="M45" s="12"/>
     </row>
     <row r="46" ht="20.05" customHeight="1">
       <c r="A46" t="s" s="10">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B46" t="s" s="11">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C46" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D46" s="13">
         <v>43875</v>
       </c>
       <c r="E46" t="s" s="14">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F46" s="12"/>
       <c r="G46" t="s" s="14">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="H46" s="12"/>
       <c r="I46" s="12"/>
       <c r="J46" s="12"/>
       <c r="K46" s="12"/>
       <c r="L46" s="12"/>
+      <c r="M46" s="12"/>
     </row>
     <row r="47" ht="20.05" customHeight="1">
       <c r="A47" t="s" s="10">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B47" t="s" s="11">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C47" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D47" s="13">
         <v>43875</v>
       </c>
       <c r="E47" t="s" s="14">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F47" s="12"/>
       <c r="G47" t="s" s="14">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="H47" s="12"/>
       <c r="I47" s="12"/>
       <c r="J47" s="12"/>
       <c r="K47" s="12"/>
       <c r="L47" s="12"/>
+      <c r="M47" s="12"/>
     </row>
     <row r="48" ht="20.05" customHeight="1">
       <c r="A48" t="s" s="10">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B48" t="s" s="11">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C48" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D48" s="13">
         <v>43875</v>
       </c>
       <c r="E48" t="s" s="14">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F48" s="12"/>
       <c r="G48" t="s" s="14">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="H48" s="12"/>
       <c r="I48" s="12"/>
       <c r="J48" s="12"/>
       <c r="K48" s="12"/>
       <c r="L48" s="12"/>
+      <c r="M48" s="12"/>
     </row>
     <row r="49" ht="20.05" customHeight="1">
       <c r="A49" t="s" s="10">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B49" t="s" s="11">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C49" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D49" s="13">
         <v>43875</v>
       </c>
       <c r="E49" t="s" s="14">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F49" s="12"/>
       <c r="G49" t="s" s="14">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="H49" s="12"/>
       <c r="I49" s="12"/>
       <c r="J49" s="12"/>
       <c r="K49" s="12"/>
       <c r="L49" s="12"/>
+      <c r="M49" s="12"/>
     </row>
     <row r="50" ht="20.05" customHeight="1">
       <c r="A50" t="s" s="10">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B50" t="s" s="11">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C50" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D50" s="13">
         <v>43875</v>
       </c>
       <c r="E50" t="s" s="14">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F50" s="12"/>
       <c r="G50" t="s" s="14">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="H50" s="12"/>
       <c r="I50" s="12"/>
       <c r="J50" s="12"/>
       <c r="K50" s="12"/>
       <c r="L50" s="12"/>
+      <c r="M50" s="12"/>
     </row>
     <row r="51" ht="20.05" customHeight="1">
       <c r="A51" t="s" s="10">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B51" t="s" s="11">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C51" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D51" s="13">
         <v>43875</v>
       </c>
       <c r="E51" t="s" s="14">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F51" s="12"/>
       <c r="G51" t="s" s="14">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="H51" s="12"/>
       <c r="I51" s="12"/>
       <c r="J51" s="12"/>
       <c r="K51" s="12"/>
       <c r="L51" s="12"/>
+      <c r="M51" s="12"/>
     </row>
     <row r="52" ht="20.05" customHeight="1">
       <c r="A52" t="s" s="10">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B52" t="s" s="11">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C52" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D52" s="13">
         <v>43875</v>
       </c>
       <c r="E52" t="s" s="14">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F52" s="12"/>
       <c r="G52" t="s" s="14">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="H52" s="12"/>
       <c r="I52" s="12"/>
       <c r="J52" s="12"/>
       <c r="K52" s="12"/>
       <c r="L52" s="12"/>
+      <c r="M52" s="12"/>
     </row>
     <row r="53" ht="20.05" customHeight="1">
       <c r="A53" t="s" s="10">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B53" t="s" s="11">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C53" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D53" s="13">
         <v>43875</v>
       </c>
       <c r="E53" t="s" s="14">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F53" s="12"/>
       <c r="G53" t="s" s="14">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="H53" s="12"/>
       <c r="I53" s="12"/>
       <c r="J53" s="12"/>
       <c r="K53" s="12"/>
       <c r="L53" s="12"/>
+      <c r="M53" s="12"/>
     </row>
     <row r="54" ht="20.05" customHeight="1">
       <c r="A54" t="s" s="10">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B54" t="s" s="11">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C54" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D54" s="13">
         <v>43888</v>
       </c>
       <c r="E54" t="s" s="14">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F54" s="12"/>
       <c r="G54" t="s" s="14">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="H54" s="12"/>
       <c r="I54" s="12"/>
       <c r="J54" s="12"/>
       <c r="K54" s="12"/>
       <c r="L54" s="12"/>
+      <c r="M54" s="12"/>
     </row>
     <row r="55" ht="20.05" customHeight="1">
       <c r="A55" t="s" s="10">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B55" t="s" s="11">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C55" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D55" s="13">
         <v>43888</v>
       </c>
       <c r="E55" t="s" s="14">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F55" s="12"/>
       <c r="G55" t="s" s="14">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="H55" s="12"/>
       <c r="I55" s="12"/>
       <c r="J55" s="12"/>
       <c r="K55" s="12"/>
       <c r="L55" s="12"/>
+      <c r="M55" s="12"/>
     </row>
     <row r="56" ht="20.05" customHeight="1">
       <c r="A56" t="s" s="10">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B56" t="s" s="11">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C56" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D56" s="13">
         <v>43875</v>
       </c>
       <c r="E56" t="s" s="14">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F56" s="12"/>
       <c r="G56" s="12"/>
       <c r="H56" s="12"/>
       <c r="I56" t="s" s="14">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="J56" s="12"/>
       <c r="K56" s="12"/>
       <c r="L56" s="12"/>
+      <c r="M56" s="12"/>
     </row>
     <row r="57" ht="20.05" customHeight="1">
       <c r="A57" t="s" s="10">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B57" t="s" s="11">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C57" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D57" s="13">
         <v>43875</v>
       </c>
       <c r="E57" t="s" s="14">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F57" s="12"/>
       <c r="G57" s="12"/>
       <c r="H57" s="12"/>
       <c r="I57" t="s" s="14">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="J57" s="12"/>
       <c r="K57" s="12"/>
       <c r="L57" s="12"/>
+      <c r="M57" s="12"/>
     </row>
     <row r="58" ht="20.05" customHeight="1">
       <c r="A58" t="s" s="10">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B58" t="s" s="11">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C58" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D58" s="13">
         <v>43875</v>
       </c>
       <c r="E58" t="s" s="14">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F58" s="12"/>
       <c r="G58" s="12"/>
       <c r="H58" s="12"/>
       <c r="I58" t="s" s="14">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="J58" s="12"/>
       <c r="K58" s="12"/>
       <c r="L58" s="12"/>
+      <c r="M58" s="12"/>
     </row>
     <row r="59" ht="20.05" customHeight="1">
       <c r="A59" t="s" s="10">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B59" t="s" s="11">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C59" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D59" s="13">
         <v>43875</v>
       </c>
       <c r="E59" t="s" s="14">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F59" s="12"/>
       <c r="G59" s="12"/>
       <c r="H59" s="12"/>
       <c r="I59" t="s" s="14">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="J59" s="12"/>
       <c r="K59" s="12"/>
       <c r="L59" s="12"/>
+      <c r="M59" s="12"/>
     </row>
     <row r="60" ht="20.05" customHeight="1">
       <c r="A60" t="s" s="10">
+        <v>117</v>
+      </c>
+      <c r="B60" t="s" s="11">
         <v>116</v>
       </c>
-      <c r="B60" t="s" s="11">
-        <v>115</v>
-      </c>
       <c r="C60" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D60" s="13">
         <v>43875</v>
       </c>
       <c r="E60" t="s" s="14">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F60" s="12"/>
       <c r="G60" s="12"/>
       <c r="H60" s="12"/>
       <c r="I60" t="s" s="14">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="J60" s="12"/>
       <c r="K60" s="12"/>
       <c r="L60" s="12"/>
+      <c r="M60" s="12"/>
     </row>
     <row r="61" ht="20.05" customHeight="1">
       <c r="A61" t="s" s="10">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B61" t="s" s="11">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C61" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D61" s="13">
         <v>43875</v>
       </c>
       <c r="E61" t="s" s="14">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F61" s="12"/>
       <c r="G61" s="12"/>
       <c r="H61" s="12"/>
       <c r="I61" t="s" s="14">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="J61" s="12"/>
       <c r="K61" s="12"/>
       <c r="L61" s="12"/>
+      <c r="M61" s="12"/>
     </row>
     <row r="62" ht="20.05" customHeight="1">
       <c r="A62" t="s" s="10">
+        <v>120</v>
+      </c>
+      <c r="B62" t="s" s="11">
         <v>119</v>
       </c>
-      <c r="B62" t="s" s="11">
-        <v>118</v>
-      </c>
       <c r="C62" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D62" s="13">
         <v>43875</v>
       </c>
       <c r="E62" t="s" s="14">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F62" s="12"/>
       <c r="G62" s="12"/>
       <c r="H62" s="12"/>
       <c r="I62" t="s" s="14">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="J62" s="12"/>
       <c r="K62" s="12"/>
       <c r="L62" s="12"/>
+      <c r="M62" s="12"/>
     </row>
     <row r="63" ht="20.05" customHeight="1">
       <c r="A63" t="s" s="10">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B63" t="s" s="11">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C63" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D63" s="13">
         <v>43875</v>
       </c>
       <c r="E63" t="s" s="14">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F63" s="12"/>
       <c r="G63" s="12"/>
       <c r="H63" s="12"/>
       <c r="I63" t="s" s="14">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="J63" s="12"/>
       <c r="K63" s="12"/>
       <c r="L63" s="12"/>
+      <c r="M63" s="12"/>
     </row>
     <row r="64" ht="20.05" customHeight="1">
       <c r="A64" t="s" s="10">
+        <v>123</v>
+      </c>
+      <c r="B64" t="s" s="11">
         <v>122</v>
       </c>
-      <c r="B64" t="s" s="11">
-        <v>121</v>
-      </c>
       <c r="C64" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D64" s="13">
         <v>43875</v>
       </c>
       <c r="E64" t="s" s="14">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F64" s="12"/>
       <c r="G64" s="12"/>
       <c r="H64" s="12"/>
       <c r="I64" t="s" s="14">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="J64" s="12"/>
       <c r="K64" s="12"/>
       <c r="L64" s="12"/>
+      <c r="M64" s="12"/>
     </row>
     <row r="65" ht="20.05" customHeight="1">
       <c r="A65" t="s" s="10">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B65" t="s" s="11">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C65" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D65" s="13">
         <v>43875</v>
       </c>
       <c r="E65" t="s" s="14">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F65" s="12"/>
       <c r="G65" s="12"/>
       <c r="H65" s="12"/>
       <c r="I65" t="s" s="14">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="J65" s="12"/>
       <c r="K65" s="12"/>
       <c r="L65" s="12"/>
+      <c r="M65" s="12"/>
     </row>
     <row r="66" ht="20.05" customHeight="1">
       <c r="A66" t="s" s="10">
+        <v>126</v>
+      </c>
+      <c r="B66" t="s" s="11">
         <v>125</v>
       </c>
-      <c r="B66" t="s" s="11">
-        <v>124</v>
-      </c>
       <c r="C66" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D66" s="13">
         <v>43888</v>
       </c>
       <c r="E66" t="s" s="14">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F66" s="12"/>
       <c r="G66" s="12"/>
       <c r="H66" s="12"/>
       <c r="I66" t="s" s="14">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="J66" s="12"/>
       <c r="K66" s="12"/>
       <c r="L66" s="12"/>
+      <c r="M66" s="12"/>
     </row>
     <row r="67" ht="20.05" customHeight="1">
       <c r="A67" t="s" s="10">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B67" t="s" s="11">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C67" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D67" s="13">
         <v>43888</v>
       </c>
       <c r="E67" t="s" s="14">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F67" s="12"/>
       <c r="G67" s="12"/>
       <c r="H67" s="12"/>
       <c r="I67" t="s" s="14">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="J67" s="12"/>
       <c r="K67" s="12"/>
       <c r="L67" s="12"/>
+      <c r="M67" s="12"/>
     </row>
     <row r="68" ht="20.05" customHeight="1">
       <c r="A68" t="s" s="10">
+        <v>129</v>
+      </c>
+      <c r="B68" t="s" s="11">
         <v>128</v>
       </c>
-      <c r="B68" t="s" s="11">
-        <v>127</v>
-      </c>
       <c r="C68" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D68" s="13">
         <v>43888</v>
       </c>
       <c r="E68" t="s" s="14">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F68" s="12"/>
       <c r="G68" s="12"/>
       <c r="H68" s="12"/>
       <c r="I68" t="s" s="14">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="J68" s="12"/>
       <c r="K68" s="12"/>
       <c r="L68" s="12"/>
+      <c r="M68" s="12"/>
     </row>
     <row r="69" ht="20.05" customHeight="1">
       <c r="A69" t="s" s="10">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B69" t="s" s="11">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C69" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D69" s="13">
         <v>43888</v>
       </c>
       <c r="E69" t="s" s="14">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F69" s="12"/>
       <c r="G69" s="12"/>
       <c r="H69" s="12"/>
       <c r="I69" t="s" s="14">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="J69" s="12"/>
       <c r="K69" s="12"/>
       <c r="L69" s="12"/>
+      <c r="M69" s="12"/>
     </row>
     <row r="70" ht="20.05" customHeight="1">
       <c r="A70" t="s" s="10">
+        <v>132</v>
+      </c>
+      <c r="B70" t="s" s="11">
         <v>131</v>
       </c>
-      <c r="B70" t="s" s="11">
-        <v>130</v>
-      </c>
       <c r="C70" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D70" s="13">
         <v>43903</v>
       </c>
       <c r="E70" t="s" s="14">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F70" s="12"/>
       <c r="G70" s="12"/>
       <c r="H70" s="12"/>
       <c r="I70" t="s" s="14">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="J70" s="12"/>
       <c r="K70" s="12"/>
       <c r="L70" s="12"/>
+      <c r="M70" s="12"/>
     </row>
     <row r="71" ht="20.05" customHeight="1">
       <c r="A71" t="s" s="10">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B71" t="s" s="11">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C71" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D71" s="13">
         <v>43903</v>
       </c>
       <c r="E71" t="s" s="14">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F71" s="12"/>
       <c r="G71" s="12"/>
       <c r="H71" s="12"/>
       <c r="I71" t="s" s="14">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="J71" s="12"/>
       <c r="K71" s="12"/>
       <c r="L71" s="12"/>
+      <c r="M71" s="12"/>
     </row>
     <row r="72" ht="20.05" customHeight="1">
       <c r="A72" t="s" s="10">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B72" t="s" s="11">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C72" t="s" s="14">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D72" s="13">
         <v>43907</v>
       </c>
       <c r="E72" t="s" s="14">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F72" s="12"/>
       <c r="G72" s="12"/>
       <c r="H72" s="12"/>
       <c r="I72" t="s" s="14">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="J72" s="12"/>
       <c r="K72" s="12"/>
       <c r="L72" s="12"/>
+      <c r="M72" s="12"/>
     </row>
     <row r="73" ht="20.05" customHeight="1">
       <c r="A73" t="s" s="10">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B73" t="s" s="11">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C73" s="12"/>
       <c r="D73" s="13">
         <v>43907</v>
       </c>
       <c r="E73" t="s" s="14">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F73" s="12"/>
       <c r="G73" s="12"/>
       <c r="H73" s="12"/>
       <c r="I73" t="s" s="14">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="J73" s="12"/>
       <c r="K73" s="12"/>
       <c r="L73" s="12"/>
+      <c r="M73" s="12"/>
     </row>
     <row r="74" ht="20.05" customHeight="1">
       <c r="A74" t="s" s="10">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B74" t="s" s="11">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C74" s="12"/>
       <c r="D74" s="13">
@@ -3630,37 +3722,39 @@
       <c r="J74" s="12"/>
       <c r="K74" s="12"/>
       <c r="L74" s="12"/>
+      <c r="M74" s="12"/>
     </row>
     <row r="75" ht="20.05" customHeight="1">
       <c r="A75" t="s" s="10">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B75" t="s" s="11">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C75" s="12"/>
       <c r="D75" s="13">
         <v>43888</v>
       </c>
       <c r="E75" t="s" s="14">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F75" s="12"/>
       <c r="G75" s="12"/>
       <c r="H75" s="12"/>
       <c r="I75" t="s" s="14">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="J75" s="12"/>
       <c r="K75" s="12"/>
       <c r="L75" s="12"/>
+      <c r="M75" s="12"/>
     </row>
     <row r="76" ht="20.05" customHeight="1">
       <c r="A76" t="s" s="10">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B76" t="s" s="11">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C76" s="12"/>
       <c r="D76" s="13">
@@ -3672,108 +3766,115 @@
       <c r="H76" s="12"/>
       <c r="I76" s="12"/>
       <c r="J76" t="s" s="14">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="K76" s="12"/>
       <c r="L76" t="s" s="14">
-        <v>145</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="M76" s="12"/>
     </row>
     <row r="77" ht="20.05" customHeight="1">
       <c r="A77" t="s" s="10">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B77" t="s" s="11">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C77" s="12"/>
       <c r="D77" s="13">
-        <v>43919</v>
+        <v>43904</v>
       </c>
       <c r="E77" t="s" s="14">
-        <v>13</v>
-      </c>
-      <c r="F77" s="12"/>
-      <c r="G77" t="s" s="14">
-        <v>17</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F77" t="s" s="14">
+        <v>9</v>
+      </c>
+      <c r="G77" s="12"/>
       <c r="H77" s="12"/>
       <c r="I77" s="12"/>
       <c r="J77" s="12"/>
       <c r="K77" s="12"/>
       <c r="L77" s="12"/>
+      <c r="M77" s="12"/>
     </row>
     <row r="78" ht="20.05" customHeight="1">
       <c r="A78" t="s" s="10">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B78" t="s" s="11">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C78" s="12"/>
       <c r="D78" s="13">
-        <v>43912</v>
+        <v>43903</v>
       </c>
       <c r="E78" t="s" s="14">
-        <v>13</v>
-      </c>
-      <c r="F78" s="12"/>
+        <v>11</v>
+      </c>
+      <c r="F78" t="s" s="14">
+        <v>9</v>
+      </c>
       <c r="G78" t="s" s="14">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="H78" s="12"/>
       <c r="I78" s="12"/>
       <c r="J78" s="12"/>
       <c r="K78" s="12"/>
       <c r="L78" s="12"/>
+      <c r="M78" s="12"/>
     </row>
     <row r="79" ht="20.05" customHeight="1">
       <c r="A79" t="s" s="10">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B79" t="s" s="11">
-        <v>151</v>
-      </c>
-      <c r="C79" t="s" s="14">
-        <v>41</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="C79" s="12"/>
       <c r="D79" s="13">
-        <v>43912</v>
+        <v>43919</v>
       </c>
       <c r="E79" t="s" s="14">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F79" s="12"/>
       <c r="G79" t="s" s="14">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="H79" s="12"/>
       <c r="I79" s="12"/>
       <c r="J79" s="12"/>
       <c r="K79" s="12"/>
       <c r="L79" s="12"/>
+      <c r="M79" s="12"/>
     </row>
     <row r="80" ht="20.05" customHeight="1">
       <c r="A80" t="s" s="10">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B80" t="s" s="11">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C80" s="12"/>
       <c r="D80" s="13">
-        <v>41424</v>
-      </c>
-      <c r="E80" s="12"/>
+        <v>43912</v>
+      </c>
+      <c r="E80" t="s" s="14">
+        <v>11</v>
+      </c>
       <c r="F80" s="12"/>
-      <c r="G80" s="12"/>
+      <c r="G80" t="s" s="14">
+        <v>52</v>
+      </c>
       <c r="H80" s="12"/>
       <c r="I80" s="12"/>
       <c r="J80" s="12"/>
-      <c r="K80" t="s" s="14">
-        <v>154</v>
-      </c>
+      <c r="K80" s="12"/>
       <c r="L80" s="12"/>
+      <c r="M80" s="12"/>
     </row>
     <row r="81" ht="20.05" customHeight="1">
       <c r="A81" t="s" s="10">
@@ -3782,47 +3883,65 @@
       <c r="B81" t="s" s="11">
         <v>156</v>
       </c>
-      <c r="C81" s="12"/>
+      <c r="C81" t="s" s="14">
+        <v>39</v>
+      </c>
       <c r="D81" s="13">
-        <v>39543</v>
-      </c>
-      <c r="E81" s="12"/>
+        <v>43912</v>
+      </c>
+      <c r="E81" t="s" s="14">
+        <v>11</v>
+      </c>
       <c r="F81" s="12"/>
-      <c r="G81" s="12"/>
+      <c r="G81" t="s" s="14">
+        <v>52</v>
+      </c>
       <c r="H81" s="12"/>
       <c r="I81" s="12"/>
       <c r="J81" s="12"/>
-      <c r="K81" t="s" s="14">
-        <v>154</v>
-      </c>
+      <c r="K81" s="12"/>
       <c r="L81" s="12"/>
+      <c r="M81" s="12"/>
     </row>
     <row r="82" ht="20.05" customHeight="1">
       <c r="A82" t="s" s="10">
         <v>157</v>
       </c>
-      <c r="B82" s="15"/>
+      <c r="B82" t="s" s="11">
+        <v>158</v>
+      </c>
       <c r="C82" s="12"/>
       <c r="D82" s="13">
-        <v>43875</v>
-      </c>
-      <c r="E82" s="12"/>
-      <c r="F82" s="12"/>
-      <c r="G82" s="12"/>
+        <v>43921</v>
+      </c>
+      <c r="E82" t="s" s="14">
+        <v>8</v>
+      </c>
+      <c r="F82" t="s" s="14">
+        <v>9</v>
+      </c>
+      <c r="G82" t="s" s="14">
+        <v>52</v>
+      </c>
       <c r="H82" s="12"/>
-      <c r="I82" s="12"/>
+      <c r="I82" t="s" s="14">
+        <v>16</v>
+      </c>
       <c r="J82" s="12"/>
       <c r="K82" s="12"/>
       <c r="L82" s="12"/>
+      <c r="M82" s="12"/>
     </row>
     <row r="83" ht="20.05" customHeight="1">
       <c r="A83" t="s" s="10">
-        <v>158</v>
-      </c>
-      <c r="B83" s="15"/>
+        <v>159</v>
+      </c>
+      <c r="B83" t="s" s="11">
+        <v>160</v>
+      </c>
       <c r="C83" s="12"/>
       <c r="D83" s="13">
-        <v>43875</v>
+        <v>41424</v>
       </c>
       <c r="E83" s="12"/>
       <c r="F83" s="12"/>
@@ -3830,17 +3949,22 @@
       <c r="H83" s="12"/>
       <c r="I83" s="12"/>
       <c r="J83" s="12"/>
-      <c r="K83" s="12"/>
+      <c r="K83" t="s" s="14">
+        <v>161</v>
+      </c>
       <c r="L83" s="12"/>
+      <c r="M83" s="12"/>
     </row>
     <row r="84" ht="20.05" customHeight="1">
       <c r="A84" t="s" s="10">
-        <v>159</v>
-      </c>
-      <c r="B84" s="15"/>
+        <v>162</v>
+      </c>
+      <c r="B84" t="s" s="11">
+        <v>163</v>
+      </c>
       <c r="C84" s="12"/>
       <c r="D84" s="13">
-        <v>43875</v>
+        <v>39543</v>
       </c>
       <c r="E84" s="12"/>
       <c r="F84" s="12"/>
@@ -3848,19 +3972,20 @@
       <c r="H84" s="12"/>
       <c r="I84" s="12"/>
       <c r="J84" s="12"/>
-      <c r="K84" s="12"/>
+      <c r="K84" t="s" s="14">
+        <v>161</v>
+      </c>
       <c r="L84" s="12"/>
+      <c r="M84" s="12"/>
     </row>
     <row r="85" ht="20.05" customHeight="1">
       <c r="A85" t="s" s="10">
-        <v>160</v>
-      </c>
-      <c r="B85" t="s" s="11">
-        <v>161</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="B85" s="15"/>
       <c r="C85" s="12"/>
       <c r="D85" s="13">
-        <v>43888</v>
+        <v>43875</v>
       </c>
       <c r="E85" s="12"/>
       <c r="F85" s="12"/>
@@ -3870,15 +3995,16 @@
       <c r="J85" s="12"/>
       <c r="K85" s="12"/>
       <c r="L85" s="12"/>
+      <c r="M85" s="12"/>
     </row>
     <row r="86" ht="20.05" customHeight="1">
       <c r="A86" t="s" s="10">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B86" s="15"/>
       <c r="C86" s="12"/>
       <c r="D86" s="13">
-        <v>43888</v>
+        <v>43875</v>
       </c>
       <c r="E86" s="12"/>
       <c r="F86" s="12"/>
@@ -3888,61 +4014,56 @@
       <c r="J86" s="12"/>
       <c r="K86" s="12"/>
       <c r="L86" s="12"/>
+      <c r="M86" s="12"/>
     </row>
     <row r="87" ht="20.05" customHeight="1">
       <c r="A87" t="s" s="10">
-        <v>163</v>
-      </c>
-      <c r="B87" t="s" s="11">
-        <v>164</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="B87" s="15"/>
       <c r="C87" s="12"/>
       <c r="D87" s="13">
-        <v>43920</v>
+        <v>43875</v>
       </c>
       <c r="E87" s="12"/>
       <c r="F87" s="12"/>
       <c r="G87" s="12"/>
-      <c r="H87" t="s" s="14">
-        <v>30</v>
-      </c>
+      <c r="H87" s="12"/>
       <c r="I87" s="12"/>
       <c r="J87" s="12"/>
       <c r="K87" s="12"/>
       <c r="L87" s="12"/>
+      <c r="M87" s="12"/>
     </row>
     <row r="88" ht="20.05" customHeight="1">
       <c r="A88" t="s" s="10">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B88" t="s" s="11">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C88" s="12"/>
       <c r="D88" s="13">
-        <v>43903</v>
+        <v>43888</v>
       </c>
       <c r="E88" s="12"/>
       <c r="F88" s="12"/>
       <c r="G88" s="12"/>
       <c r="H88" s="12"/>
       <c r="I88" s="12"/>
-      <c r="J88" t="s" s="14">
-        <v>144</v>
-      </c>
+      <c r="J88" s="12"/>
       <c r="K88" s="12"/>
       <c r="L88" s="12"/>
+      <c r="M88" s="12"/>
     </row>
     <row r="89" ht="20.05" customHeight="1">
       <c r="A89" t="s" s="10">
-        <v>167</v>
-      </c>
-      <c r="B89" t="s" s="11">
-        <v>168</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="B89" s="15"/>
       <c r="C89" s="12"/>
       <c r="D89" s="13">
-        <v>43920</v>
+        <v>43888</v>
       </c>
       <c r="E89" s="12"/>
       <c r="F89" s="12"/>
@@ -3952,10 +4073,57 @@
       <c r="J89" s="12"/>
       <c r="K89" s="12"/>
       <c r="L89" s="12"/>
+      <c r="M89" s="12"/>
+    </row>
+    <row r="90" ht="20.05" customHeight="1">
+      <c r="A90" t="s" s="10">
+        <v>170</v>
+      </c>
+      <c r="B90" t="s" s="11">
+        <v>171</v>
+      </c>
+      <c r="C90" s="12"/>
+      <c r="D90" s="13">
+        <v>43920</v>
+      </c>
+      <c r="E90" s="12"/>
+      <c r="F90" s="12"/>
+      <c r="G90" s="12"/>
+      <c r="H90" t="s" s="14">
+        <v>26</v>
+      </c>
+      <c r="I90" s="12"/>
+      <c r="J90" s="12"/>
+      <c r="K90" s="12"/>
+      <c r="L90" s="12"/>
+      <c r="M90" s="12"/>
+    </row>
+    <row r="91" ht="20.05" customHeight="1">
+      <c r="A91" t="s" s="10">
+        <v>172</v>
+      </c>
+      <c r="B91" t="s" s="11">
+        <v>173</v>
+      </c>
+      <c r="C91" s="12"/>
+      <c r="D91" s="13">
+        <v>43903</v>
+      </c>
+      <c r="E91" s="12"/>
+      <c r="F91" s="12"/>
+      <c r="G91" s="12"/>
+      <c r="H91" s="12"/>
+      <c r="I91" s="12"/>
+      <c r="J91" t="s" s="14">
+        <v>145</v>
+      </c>
+      <c r="K91" s="12"/>
+      <c r="L91" s="12"/>
+      <c r="M91" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A1:M1"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>